<commit_message>
Update holiday hours and menu items in all you can eat
</commit_message>
<xml_diff>
--- a/src/assets/menu/menu.xlsx
+++ b/src/assets/menu/menu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/translucenttree/Coding/business/sushi-ai/src/assets/menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0D4E1-B2C2-3940-9E1F-06CEA763609A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE116677-A2D6-D147-9757-63900AE66782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dishes" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="423">
   <si>
     <t>order</t>
   </si>
@@ -643,9 +643,6 @@
     <t>Tempura Oreo (5)</t>
   </si>
   <si>
-    <t>Deep fried oreo cookies wit tempura breading and whipped cream</t>
-  </si>
-  <si>
     <t>Bento Box</t>
   </si>
   <si>
@@ -1156,9 +1153,6 @@
     <t>Yellowtail</t>
   </si>
   <si>
-    <t>Ika Salad</t>
-  </si>
-  <si>
     <t>Salmon, cream cheese, and scallions</t>
   </si>
   <si>
@@ -1276,9 +1270,6 @@
     <t>Shrimp tempura, cucumber, and avocado topped with crunch</t>
   </si>
   <si>
-    <t>Mango</t>
-  </si>
-  <si>
     <t>Green Tea</t>
   </si>
   <si>
@@ -1298,6 +1289,9 @@
   </si>
   <si>
     <t>Served with 6 pieces of California Roll, vegetable tempura, shumai, crab rangoon, spring roll, white rice, salad, and miso soup. Substitute with fried rice for $2.95.</t>
+  </si>
+  <si>
+    <t>Deep fried oreo cookies with tempura breading and whipped cream</t>
   </si>
 </sst>
 </file>
@@ -1595,8 +1589,8 @@
   </sheetPr>
   <dimension ref="A1:E1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3687,7 +3681,7 @@
         <v>188</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D135" s="2">
         <v>14.95</v>
@@ -3814,7 +3808,7 @@
         <v>5.95</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>206</v>
+        <v>422</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -3822,7 +3816,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>189</v>
@@ -3836,7 +3830,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>164</v>
@@ -3850,7 +3844,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>190</v>
@@ -3864,7 +3858,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>165</v>
@@ -3878,7 +3872,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>191</v>
@@ -3892,7 +3886,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>166</v>
@@ -3906,7 +3900,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>192</v>
@@ -3920,7 +3914,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>167</v>
@@ -3934,7 +3928,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>193</v>
@@ -3948,7 +3942,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>194</v>
@@ -3962,7 +3956,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>197</v>
@@ -3979,7 +3973,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>30</v>
@@ -3993,7 +3987,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>173</v>
@@ -4007,7 +4001,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>141</v>
@@ -4021,7 +4015,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>138</v>
@@ -4035,7 +4029,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>50</v>
@@ -4049,10 +4043,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C160" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D160" s="2">
         <v>14.95</v>
@@ -4063,7 +4057,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>139</v>
@@ -4077,7 +4071,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>141</v>
@@ -4091,7 +4085,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>30</v>
@@ -4105,7 +4099,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>138</v>
@@ -4119,10 +4113,10 @@
         <v>164</v>
       </c>
       <c r="B165" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="D165" s="2">
         <v>15.95</v>
@@ -4133,7 +4127,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>139</v>
@@ -4147,7 +4141,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>50</v>
@@ -4161,16 +4155,16 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C168" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="D168" s="2">
         <v>12.95</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4178,16 +4172,16 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D169" s="2">
         <v>14.95</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4195,16 +4189,16 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D170" s="2">
         <v>14.75</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4212,16 +4206,16 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D171" s="2">
         <v>14.95</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4229,16 +4223,16 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D172" s="2">
         <v>12.55</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4246,16 +4240,16 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D173" s="2">
         <v>14.75</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4263,16 +4257,16 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D174" s="2">
         <v>14.55</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4280,16 +4274,16 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D175" s="2">
         <v>15.75</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4297,16 +4291,16 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D176" s="2">
         <v>14.75</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4314,16 +4308,16 @@
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D177" s="2">
         <v>14.75</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4331,16 +4325,16 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D178" s="2">
         <v>12.95</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4348,16 +4342,16 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D179" s="2">
         <v>12.95</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4365,16 +4359,16 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D180" s="2">
         <v>15.95</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4382,16 +4376,16 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D181" s="2">
         <v>15.95</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4399,16 +4393,16 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D182" s="2">
         <v>16.95</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4416,16 +4410,16 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D183" s="2">
         <v>13.85</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4433,16 +4427,16 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D184" s="2">
         <v>14.95</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4450,16 +4444,16 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D185" s="2">
         <v>13.49</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4467,16 +4461,16 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D186" s="2">
         <v>29.95</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4484,16 +4478,16 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D187" s="3">
         <v>19.95</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4501,16 +4495,16 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D188" s="2">
         <v>12.49</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4518,16 +4512,16 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D189" s="2">
         <v>13.49</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4535,16 +4529,16 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D190" s="2">
         <v>12.95</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4552,16 +4546,16 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D191" s="2">
         <v>12.95</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4569,16 +4563,16 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D192" s="2">
         <v>13.95</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4586,16 +4580,16 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C193" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="D193" s="2">
         <v>9.9499999999999993</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4603,16 +4597,16 @@
         <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D194" s="2">
         <v>10.95</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4620,16 +4614,16 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D195" s="5">
         <v>11.95</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4637,16 +4631,16 @@
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D196" s="5">
         <v>10.75</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4654,16 +4648,16 @@
         <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D197" s="5">
         <v>10.55</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4671,16 +4665,16 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D198" s="5">
         <v>10.55</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4688,16 +4682,16 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D199" s="5">
         <v>10.49</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4705,16 +4699,16 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D200" s="5">
         <v>10.49</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4722,16 +4716,16 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D201" s="5">
         <v>10.49</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4739,16 +4733,16 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D202" s="5">
         <v>10.55</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4756,16 +4750,16 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D203" s="5">
         <v>10.49</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4773,16 +4767,16 @@
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D204" s="5">
         <v>10.95</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4790,16 +4784,16 @@
         <v>204</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D205" s="5">
         <v>12.49</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -7252,7 +7246,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -7266,7 +7260,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7277,7 +7271,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7288,10 +7282,10 @@
         <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7302,7 +7296,7 @@
         <v>79</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7313,10 +7307,10 @@
         <v>137</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7327,10 +7321,10 @@
         <v>146</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7341,10 +7335,10 @@
         <v>163</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7355,10 +7349,10 @@
         <v>168</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7369,10 +7363,10 @@
         <v>172</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7383,7 +7377,7 @@
         <v>176</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7394,7 +7388,7 @@
         <v>183</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7405,10 +7399,10 @@
         <v>188</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7419,7 +7413,7 @@
         <v>199</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7427,13 +7421,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7441,10 +7435,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7452,13 +7446,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7466,10 +7460,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7477,10 +7471,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7488,10 +7482,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7499,10 +7493,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7510,10 +7504,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7521,10 +7515,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7532,10 +7526,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7543,10 +7537,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7554,10 +7548,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7565,10 +7559,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7576,10 +7570,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7587,10 +7581,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7598,10 +7592,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7609,10 +7603,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7620,10 +7614,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7631,10 +7625,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7642,10 +7636,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7656,7 +7650,7 @@
         <v>203</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -7671,7 +7665,9 @@
   </sheetPr>
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7691,7 +7687,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -7702,7 +7698,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -7713,7 +7709,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -7724,10 +7720,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7735,10 +7731,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7746,10 +7742,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7757,10 +7753,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7768,10 +7764,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7779,10 +7775,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7790,10 +7786,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7801,7 +7797,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>50</v>
@@ -7812,7 +7808,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>52</v>
@@ -7823,7 +7819,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>56</v>
@@ -7834,7 +7830,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>69</v>
@@ -7845,7 +7841,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -7856,10 +7852,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7867,10 +7863,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7878,13 +7874,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7892,13 +7888,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7906,13 +7902,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7920,13 +7916,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7934,13 +7930,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7948,13 +7944,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7962,13 +7958,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7976,10 +7972,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7987,16 +7983,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8004,13 +8000,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8018,16 +8014,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8035,16 +8031,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8052,13 +8048,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8066,10 +8062,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8077,13 +8073,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8091,13 +8087,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8105,10 +8101,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8116,10 +8112,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8127,13 +8123,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8141,13 +8137,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8155,10 +8151,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8166,13 +8162,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8180,10 +8176,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8191,13 +8187,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8205,10 +8201,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8216,13 +8212,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8230,13 +8226,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8244,16 +8240,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8261,13 +8257,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8275,13 +8271,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8289,10 +8285,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8300,13 +8296,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8314,16 +8310,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8331,13 +8327,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8345,16 +8341,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8362,13 +8358,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8376,13 +8372,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8390,16 +8386,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8407,13 +8403,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -8421,13 +8417,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -8442,7 +8438,9 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8462,7 +8460,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -8473,7 +8471,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -8484,7 +8482,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -8495,10 +8493,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8506,10 +8504,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8517,10 +8515,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8528,10 +8526,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8539,10 +8537,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8550,10 +8548,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8561,10 +8559,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8572,10 +8570,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8583,10 +8581,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8594,10 +8592,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8605,10 +8603,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8616,10 +8614,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8627,10 +8625,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8638,10 +8636,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8649,10 +8647,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8660,10 +8658,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8671,10 +8669,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8682,10 +8680,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8693,7 +8691,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>52</v>
@@ -8704,13 +8702,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8718,7 +8716,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>56</v>
@@ -8729,10 +8727,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8740,7 +8738,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>62</v>
@@ -8751,7 +8749,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>69</v>
@@ -8762,13 +8760,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8776,13 +8774,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8790,7 +8788,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>15</v>
@@ -8801,13 +8799,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8815,13 +8813,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8829,13 +8827,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8843,13 +8841,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8857,7 +8855,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>50</v>
@@ -8868,13 +8866,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8882,10 +8880,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8893,13 +8891,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8907,7 +8905,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>30</v>
@@ -8918,13 +8916,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8932,7 +8930,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>77</v>
@@ -8943,10 +8941,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>377</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8954,10 +8952,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8968,10 +8969,13 @@
         <v>305</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>66</v>
+        <v>319</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8979,13 +8983,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>318</v>
+        <v>377</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>378</v>
@@ -8996,13 +8997,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>379</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9010,13 +9011,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9024,13 +9025,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9038,13 +9039,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>383</v>
+        <v>102</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9052,13 +9053,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>102</v>
+        <v>353</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9066,13 +9067,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>385</v>
+        <v>318</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9080,10 +9078,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>319</v>
+        <v>114</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9091,13 +9092,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>114</v>
+        <v>375</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9105,13 +9106,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>376</v>
+        <v>42</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9119,13 +9120,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>42</v>
+        <v>384</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9133,16 +9137,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>386</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9150,16 +9154,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>318</v>
+        <v>323</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>388</v>
+        <v>324</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9167,16 +9171,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>318</v>
+        <v>387</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>317</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>325</v>
+        <v>388</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9184,16 +9188,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9201,13 +9202,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9215,16 +9219,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>273</v>
+        <v>391</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9232,9 +9230,15 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>393</v>
       </c>
     </row>
@@ -9243,16 +9247,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>395</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9260,10 +9258,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9271,10 +9269,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9282,10 +9280,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>338</v>
+        <v>361</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9293,16 +9297,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9310,10 +9308,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9321,10 +9319,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>336</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9332,10 +9330,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>127</v>
+        <v>359</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9343,13 +9344,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>360</v>
+        <v>328</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>396</v>
+        <v>329</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9357,13 +9358,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>330</v>
+        <v>395</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9371,13 +9372,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>397</v>
+        <v>141</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9385,13 +9386,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9399,13 +9400,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9413,10 +9411,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>399</v>
+        <v>341</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9424,13 +9425,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9438,10 +9436,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>352</v>
+        <v>76</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9449,13 +9450,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>318</v>
+        <v>398</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9466,13 +9470,7 @@
         <v>306</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>401</v>
+        <v>349</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9480,10 +9478,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>350</v>
+        <v>400</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9491,16 +9495,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>402</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9508,13 +9509,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>262</v>
+        <v>343</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9522,16 +9526,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>318</v>
+        <v>131</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>405</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9539,13 +9540,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>131</v>
+        <v>404</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>340</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9553,13 +9554,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E86" s="4" t="s">
         <v>406</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9567,10 +9568,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>232</v>
+        <v>407</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>408</v>
@@ -9581,16 +9585,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="E88" s="4" t="s">
-        <v>410</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9598,13 +9599,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C89" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9612,7 +9613,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>412</v>
@@ -9626,13 +9627,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>414</v>
+        <v>135</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>415</v>
+        <v>350</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9640,13 +9641,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -9654,61 +9655,42 @@
         <v>92</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>348</v>
+        <v>263</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>349</v>
+        <v>414</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>93</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>416</v>
+      <c r="B94" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>94</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C95" s="4" t="s">
-        <v>417</v>
+      <c r="C95" s="1" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A96" s="1">
-        <v>95</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A97" s="1">
-        <v>96</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>419</v>
-      </c>
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A97" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>